<commit_message>
feat: ajuste do ranking
</commit_message>
<xml_diff>
--- a/docs/Ranking N2BT.xlsx
+++ b/docs/Ranking N2BT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\leguass7\@n2bt\n2bt-next\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\1 Resenha Open Speed\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking N2BT" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="226">
   <si>
     <t>50+ Masculino</t>
   </si>
@@ -560,15 +560,33 @@
     <t>Marina Haydne</t>
   </si>
   <si>
+    <t>Kardeny</t>
+  </si>
+  <si>
+    <t>Ticiana</t>
+  </si>
+  <si>
+    <t>Priscila</t>
+  </si>
+  <si>
+    <t>Mariana</t>
+  </si>
+  <si>
     <t>Andre</t>
   </si>
   <si>
     <t>Ceane</t>
   </si>
   <si>
+    <t>Liliana</t>
+  </si>
+  <si>
     <t>Malu</t>
   </si>
   <si>
+    <t>Marcia</t>
+  </si>
+  <si>
     <t>Laryssa</t>
   </si>
   <si>
@@ -684,37 +702,13 @@
   </si>
   <si>
     <t>3ª</t>
-  </si>
-  <si>
-    <t>Ticiana Nayara</t>
-  </si>
-  <si>
-    <t>Kardeny Sales</t>
-  </si>
-  <si>
-    <t>Priscila Batista</t>
-  </si>
-  <si>
-    <t>Mariana Martins</t>
-  </si>
-  <si>
-    <t>Liliana Moraes</t>
-  </si>
-  <si>
-    <t>Marcia Medeiros</t>
-  </si>
-  <si>
-    <t>Juliana Sá</t>
-  </si>
-  <si>
-    <t>Leandro Oliveira</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -722,37 +716,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -764,19 +734,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bom" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutra" xfId="2" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1057,37 +1021,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AZ1" sqref="AZ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="4" customWidth="1"/>
     <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="4" customWidth="1"/>
     <col min="19" max="19" width="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="4" customWidth="1"/>
     <col min="25" max="25" width="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
     <col min="28" max="30" width="4" customWidth="1"/>
     <col min="31" max="31" width="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="4" bestFit="1" customWidth="1"/>
     <col min="34" max="37" width="4" customWidth="1"/>
-    <col min="38" max="38" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="4" bestFit="1" customWidth="1"/>
     <col min="40" max="43" width="4" customWidth="1"/>
     <col min="44" max="44" width="16" bestFit="1" customWidth="1"/>
@@ -1095,109 +1059,109 @@
     <col min="46" max="47" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="J1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="K1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="N1" t="s">
         <v>0</v>
       </c>
       <c r="O1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="P1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="Q1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="T1" t="s">
         <v>4</v>
       </c>
       <c r="U1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="V1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="W1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="Z1" t="s">
         <v>5</v>
       </c>
       <c r="AA1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="AB1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="AC1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="AF1" t="s">
         <v>2</v>
       </c>
       <c r="AG1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="AH1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="AI1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="AL1" t="s">
         <v>3</v>
       </c>
       <c r="AM1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="AN1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="AO1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="AR1" t="s">
         <v>6</v>
       </c>
       <c r="AS1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="AT1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="AU1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2">
@@ -1207,7 +1171,7 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>59</v>
       </c>
       <c r="I2">
@@ -1217,7 +1181,7 @@
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>60</v>
       </c>
       <c r="O2">
@@ -1227,7 +1191,7 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" t="s">
         <v>100</v>
       </c>
       <c r="U2">
@@ -1237,7 +1201,7 @@
       <c r="AE2">
         <v>1</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AF2" t="s">
         <v>135</v>
       </c>
       <c r="AG2">
@@ -1247,7 +1211,7 @@
       <c r="AK2">
         <v>1</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AL2" t="s">
         <v>151</v>
       </c>
       <c r="AM2">
@@ -1257,7 +1221,7 @@
       <c r="AQ2">
         <v>1</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AR2" t="s">
         <v>168</v>
       </c>
       <c r="AS2">
@@ -1265,11 +1229,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3">
@@ -1279,7 +1243,7 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>31</v>
       </c>
       <c r="I3">
@@ -1289,7 +1253,7 @@
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" t="s">
         <v>75</v>
       </c>
       <c r="O3">
@@ -1299,7 +1263,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" t="s">
         <v>101</v>
       </c>
       <c r="U3">
@@ -1309,7 +1273,7 @@
       <c r="AE3">
         <v>1</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AF3" t="s">
         <v>136</v>
       </c>
       <c r="AG3">
@@ -1329,7 +1293,7 @@
       <c r="AQ3">
         <v>1</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AR3" t="s">
         <v>169</v>
       </c>
       <c r="AS3">
@@ -1337,11 +1301,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4">
@@ -1351,7 +1315,7 @@
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>60</v>
       </c>
       <c r="I4">
@@ -1361,7 +1325,7 @@
       <c r="M4">
         <v>2</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" t="s">
         <v>80</v>
       </c>
       <c r="O4">
@@ -1371,7 +1335,7 @@
       <c r="S4">
         <v>2</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" t="s">
         <v>102</v>
       </c>
       <c r="U4">
@@ -1381,7 +1345,7 @@
       <c r="AE4">
         <v>2</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AF4" t="s">
         <v>137</v>
       </c>
       <c r="AG4">
@@ -1391,7 +1355,7 @@
       <c r="AK4">
         <v>2</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AL4" t="s">
         <v>149</v>
       </c>
       <c r="AM4">
@@ -1401,7 +1365,7 @@
       <c r="AQ4">
         <v>2</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AR4" t="s">
         <v>170</v>
       </c>
       <c r="AS4">
@@ -1409,11 +1373,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5">
@@ -1423,7 +1387,7 @@
       <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>61</v>
       </c>
       <c r="I5">
@@ -1433,7 +1397,7 @@
       <c r="M5">
         <v>2</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" t="s">
         <v>81</v>
       </c>
       <c r="O5">
@@ -1443,7 +1407,7 @@
       <c r="S5">
         <v>2</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" t="s">
         <v>100</v>
       </c>
       <c r="U5">
@@ -1453,7 +1417,7 @@
       <c r="AE5">
         <v>2</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AF5" t="s">
         <v>138</v>
       </c>
       <c r="AG5">
@@ -1463,7 +1427,7 @@
       <c r="AK5">
         <v>2</v>
       </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AL5" t="s">
         <v>150</v>
       </c>
       <c r="AM5">
@@ -1473,7 +1437,7 @@
       <c r="AQ5">
         <v>2</v>
       </c>
-      <c r="AR5" s="1" t="s">
+      <c r="AR5" t="s">
         <v>171</v>
       </c>
       <c r="AS5">
@@ -1481,11 +1445,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6">
@@ -1495,7 +1459,7 @@
       <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>62</v>
       </c>
       <c r="I6">
@@ -1505,7 +1469,7 @@
       <c r="M6">
         <v>3</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" t="s">
         <v>82</v>
       </c>
       <c r="O6">
@@ -1525,7 +1489,7 @@
       <c r="AE6">
         <v>3</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AF6" t="s">
         <v>139</v>
       </c>
       <c r="AG6">
@@ -1535,7 +1499,7 @@
       <c r="AK6">
         <v>3</v>
       </c>
-      <c r="AL6" s="1" t="s">
+      <c r="AL6" t="s">
         <v>148</v>
       </c>
       <c r="AM6">
@@ -1545,7 +1509,7 @@
       <c r="AQ6">
         <v>3</v>
       </c>
-      <c r="AR6" s="1" t="s">
+      <c r="AR6" t="s">
         <v>172</v>
       </c>
       <c r="AS6">
@@ -1553,11 +1517,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7">
@@ -1567,7 +1531,7 @@
       <c r="G7">
         <v>3</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>63</v>
       </c>
       <c r="I7">
@@ -1577,7 +1541,7 @@
       <c r="M7">
         <v>3</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" t="s">
         <v>83</v>
       </c>
       <c r="O7">
@@ -1597,7 +1561,7 @@
       <c r="AE7">
         <v>3</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AF7" t="s">
         <v>140</v>
       </c>
       <c r="AG7">
@@ -1607,7 +1571,7 @@
       <c r="AK7">
         <v>3</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AL7" t="s">
         <v>153</v>
       </c>
       <c r="AM7">
@@ -1617,7 +1581,7 @@
       <c r="AQ7">
         <v>3</v>
       </c>
-      <c r="AR7" s="1" t="s">
+      <c r="AR7" t="s">
         <v>173</v>
       </c>
       <c r="AS7">
@@ -1625,7 +1589,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1639,7 +1603,7 @@
       <c r="G8">
         <v>3</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>64</v>
       </c>
       <c r="I8">
@@ -1649,7 +1613,7 @@
       <c r="M8">
         <v>3</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" t="s">
         <v>84</v>
       </c>
       <c r="O8">
@@ -1669,7 +1633,7 @@
       <c r="AE8">
         <v>3</v>
       </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AF8" t="s">
         <v>141</v>
       </c>
       <c r="AG8">
@@ -1679,7 +1643,7 @@
       <c r="AK8">
         <v>3</v>
       </c>
-      <c r="AL8" s="1" t="s">
+      <c r="AL8" t="s">
         <v>143</v>
       </c>
       <c r="AM8">
@@ -1689,7 +1653,7 @@
       <c r="AQ8">
         <v>3</v>
       </c>
-      <c r="AR8" s="1" t="s">
+      <c r="AR8" t="s">
         <v>174</v>
       </c>
       <c r="AS8">
@@ -1697,7 +1661,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1711,7 +1675,7 @@
       <c r="G9">
         <v>3</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>65</v>
       </c>
       <c r="I9">
@@ -1721,7 +1685,7 @@
       <c r="M9">
         <v>3</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" t="s">
         <v>85</v>
       </c>
       <c r="O9">
@@ -1741,7 +1705,7 @@
       <c r="AE9">
         <v>3</v>
       </c>
-      <c r="AF9" s="1" t="s">
+      <c r="AF9" t="s">
         <v>142</v>
       </c>
       <c r="AG9">
@@ -1751,7 +1715,7 @@
       <c r="AK9">
         <v>3</v>
       </c>
-      <c r="AL9" s="1" t="s">
+      <c r="AL9" t="s">
         <v>154</v>
       </c>
       <c r="AM9">
@@ -1761,7 +1725,7 @@
       <c r="AQ9">
         <v>3</v>
       </c>
-      <c r="AR9" s="1" t="s">
+      <c r="AR9" t="s">
         <v>175</v>
       </c>
       <c r="AS9">
@@ -1769,11 +1733,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10">
@@ -1783,7 +1747,7 @@
       <c r="G10">
         <v>5</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>66</v>
       </c>
       <c r="I10">
@@ -1793,7 +1757,7 @@
       <c r="M10">
         <v>5</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" t="s">
         <v>44</v>
       </c>
       <c r="O10">
@@ -1803,7 +1767,7 @@
       <c r="S10">
         <v>5</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" t="s">
         <v>51</v>
       </c>
       <c r="U10">
@@ -1813,7 +1777,7 @@
       <c r="AE10">
         <v>5</v>
       </c>
-      <c r="AF10" s="1" t="s">
+      <c r="AF10" t="s">
         <v>143</v>
       </c>
       <c r="AG10">
@@ -1823,7 +1787,7 @@
       <c r="AK10">
         <v>5</v>
       </c>
-      <c r="AL10" s="1" t="s">
+      <c r="AL10" t="s">
         <v>155</v>
       </c>
       <c r="AM10">
@@ -1841,11 +1805,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11">
@@ -1855,7 +1819,7 @@
       <c r="G11">
         <v>5</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>67</v>
       </c>
       <c r="I11">
@@ -1865,7 +1829,7 @@
       <c r="M11">
         <v>5</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N11" t="s">
         <v>86</v>
       </c>
       <c r="O11">
@@ -1875,7 +1839,7 @@
       <c r="S11">
         <v>5</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" t="s">
         <v>106</v>
       </c>
       <c r="U11">
@@ -1885,7 +1849,7 @@
       <c r="AE11">
         <v>5</v>
       </c>
-      <c r="AF11" s="1" t="s">
+      <c r="AF11" t="s">
         <v>144</v>
       </c>
       <c r="AG11">
@@ -1895,7 +1859,7 @@
       <c r="AK11">
         <v>5</v>
       </c>
-      <c r="AL11" s="1" t="s">
+      <c r="AL11" t="s">
         <v>147</v>
       </c>
       <c r="AM11">
@@ -1913,11 +1877,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12">
@@ -1927,7 +1891,7 @@
       <c r="G12">
         <v>5</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
         <v>68</v>
       </c>
       <c r="I12">
@@ -1937,7 +1901,7 @@
       <c r="M12">
         <v>5</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N12" t="s">
         <v>87</v>
       </c>
       <c r="O12">
@@ -1947,7 +1911,7 @@
       <c r="S12">
         <v>5</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="T12" t="s">
         <v>41</v>
       </c>
       <c r="U12">
@@ -1957,7 +1921,7 @@
       <c r="AE12">
         <v>5</v>
       </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AF12" t="s">
         <v>145</v>
       </c>
       <c r="AG12">
@@ -1967,7 +1931,7 @@
       <c r="AK12">
         <v>5</v>
       </c>
-      <c r="AL12" s="1" t="s">
+      <c r="AL12" t="s">
         <v>156</v>
       </c>
       <c r="AM12">
@@ -1977,19 +1941,19 @@
       <c r="AQ12">
         <v>5</v>
       </c>
-      <c r="AR12" s="1" t="s">
-        <v>221</v>
+      <c r="AR12" t="s">
+        <v>178</v>
       </c>
       <c r="AS12">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="C13">
@@ -1999,7 +1963,7 @@
       <c r="G13">
         <v>5</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" t="s">
         <v>69</v>
       </c>
       <c r="I13">
@@ -2009,7 +1973,7 @@
       <c r="M13">
         <v>5</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N13" t="s">
         <v>88</v>
       </c>
       <c r="O13">
@@ -2019,7 +1983,7 @@
       <c r="S13">
         <v>5</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="T13" t="s">
         <v>107</v>
       </c>
       <c r="U13">
@@ -2029,7 +1993,7 @@
       <c r="AE13">
         <v>5</v>
       </c>
-      <c r="AF13" s="1" t="s">
+      <c r="AF13" t="s">
         <v>146</v>
       </c>
       <c r="AG13">
@@ -2039,7 +2003,7 @@
       <c r="AK13">
         <v>5</v>
       </c>
-      <c r="AL13" s="1" t="s">
+      <c r="AL13" t="s">
         <v>157</v>
       </c>
       <c r="AM13">
@@ -2049,19 +2013,19 @@
       <c r="AQ13">
         <v>5</v>
       </c>
-      <c r="AR13" s="1" t="s">
-        <v>220</v>
+      <c r="AR13" t="s">
+        <v>179</v>
       </c>
       <c r="AS13">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14">
@@ -2071,7 +2035,7 @@
       <c r="G14">
         <v>5</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" t="s">
         <v>70</v>
       </c>
       <c r="I14">
@@ -2081,7 +2045,7 @@
       <c r="M14">
         <v>5</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="N14" t="s">
         <v>89</v>
       </c>
       <c r="O14">
@@ -2091,7 +2055,7 @@
       <c r="S14">
         <v>5</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="T14" t="s">
         <v>108</v>
       </c>
       <c r="U14">
@@ -2101,7 +2065,7 @@
       <c r="AE14">
         <v>5</v>
       </c>
-      <c r="AF14" s="1" t="s">
+      <c r="AF14" t="s">
         <v>147</v>
       </c>
       <c r="AG14">
@@ -2111,7 +2075,7 @@
       <c r="AK14">
         <v>5</v>
       </c>
-      <c r="AL14" s="1" t="s">
+      <c r="AL14" t="s">
         <v>146</v>
       </c>
       <c r="AM14">
@@ -2121,19 +2085,19 @@
       <c r="AQ14">
         <v>5</v>
       </c>
-      <c r="AR14" s="1" t="s">
-        <v>222</v>
+      <c r="AR14" t="s">
+        <v>180</v>
       </c>
       <c r="AS14">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15">
@@ -2143,7 +2107,7 @@
       <c r="G15">
         <v>5</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" t="s">
         <v>71</v>
       </c>
       <c r="I15">
@@ -2153,7 +2117,7 @@
       <c r="M15">
         <v>5</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="N15" t="s">
         <v>90</v>
       </c>
       <c r="O15">
@@ -2163,8 +2127,8 @@
       <c r="S15">
         <v>5</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>227</v>
+      <c r="T15" t="s">
+        <v>59</v>
       </c>
       <c r="U15">
         <f t="shared" si="3"/>
@@ -2173,7 +2137,7 @@
       <c r="AE15">
         <v>5</v>
       </c>
-      <c r="AF15" s="1" t="s">
+      <c r="AF15" t="s">
         <v>148</v>
       </c>
       <c r="AG15">
@@ -2183,7 +2147,7 @@
       <c r="AK15">
         <v>5</v>
       </c>
-      <c r="AL15" s="1" t="s">
+      <c r="AL15" t="s">
         <v>140</v>
       </c>
       <c r="AM15">
@@ -2193,19 +2157,19 @@
       <c r="AQ15">
         <v>5</v>
       </c>
-      <c r="AR15" s="1" t="s">
-        <v>223</v>
+      <c r="AR15" t="s">
+        <v>181</v>
       </c>
       <c r="AS15">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>22</v>
       </c>
       <c r="C16">
@@ -2215,7 +2179,7 @@
       <c r="G16">
         <v>5</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" t="s">
         <v>72</v>
       </c>
       <c r="I16">
@@ -2225,7 +2189,7 @@
       <c r="M16">
         <v>5</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="N16" t="s">
         <v>91</v>
       </c>
       <c r="O16">
@@ -2245,7 +2209,7 @@
       <c r="AE16">
         <v>5</v>
       </c>
-      <c r="AF16" s="1" t="s">
+      <c r="AF16" t="s">
         <v>149</v>
       </c>
       <c r="AG16">
@@ -2255,7 +2219,7 @@
       <c r="AK16">
         <v>5</v>
       </c>
-      <c r="AL16" s="1" t="s">
+      <c r="AL16" t="s">
         <v>158</v>
       </c>
       <c r="AM16">
@@ -2265,19 +2229,19 @@
       <c r="AQ16">
         <v>5</v>
       </c>
-      <c r="AR16" s="1" t="s">
-        <v>178</v>
+      <c r="AR16" t="s">
+        <v>182</v>
       </c>
       <c r="AS16">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="C17">
@@ -2287,7 +2251,7 @@
       <c r="G17">
         <v>5</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" t="s">
         <v>10</v>
       </c>
       <c r="I17">
@@ -2297,7 +2261,7 @@
       <c r="M17">
         <v>5</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="N17" t="s">
         <v>92</v>
       </c>
       <c r="O17">
@@ -2307,7 +2271,7 @@
       <c r="S17">
         <v>5</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="T17" t="s">
         <v>109</v>
       </c>
       <c r="U17">
@@ -2317,7 +2281,7 @@
       <c r="AE17">
         <v>5</v>
       </c>
-      <c r="AF17" s="1" t="s">
+      <c r="AF17" t="s">
         <v>150</v>
       </c>
       <c r="AG17">
@@ -2327,7 +2291,7 @@
       <c r="AK17">
         <v>5</v>
       </c>
-      <c r="AL17" s="1" t="s">
+      <c r="AL17" t="s">
         <v>159</v>
       </c>
       <c r="AM17">
@@ -2337,19 +2301,19 @@
       <c r="AQ17">
         <v>5</v>
       </c>
-      <c r="AR17" s="1" t="s">
-        <v>179</v>
+      <c r="AR17" t="s">
+        <v>183</v>
       </c>
       <c r="AS17">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="C18">
@@ -2359,7 +2323,7 @@
       <c r="G18">
         <v>9</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>73</v>
       </c>
       <c r="I18">
@@ -2369,7 +2333,7 @@
       <c r="M18">
         <v>9</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="N18" t="s">
         <v>93</v>
       </c>
       <c r="O18">
@@ -2379,7 +2343,7 @@
       <c r="S18">
         <v>9</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="T18" t="s">
         <v>110</v>
       </c>
       <c r="U18">
@@ -2389,7 +2353,7 @@
       <c r="AK18">
         <v>9</v>
       </c>
-      <c r="AL18" s="1" t="s">
+      <c r="AL18" t="s">
         <v>166</v>
       </c>
       <c r="AM18">
@@ -2399,19 +2363,19 @@
       <c r="AQ18">
         <v>9</v>
       </c>
-      <c r="AR18" s="1" t="s">
-        <v>224</v>
+      <c r="AR18" t="s">
+        <v>184</v>
       </c>
       <c r="AS18">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>9</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>25</v>
       </c>
       <c r="C19">
@@ -2421,7 +2385,7 @@
       <c r="G19">
         <v>9</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" t="s">
         <v>74</v>
       </c>
       <c r="I19">
@@ -2431,7 +2395,7 @@
       <c r="M19">
         <v>9</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="N19" t="s">
         <v>94</v>
       </c>
       <c r="O19">
@@ -2441,7 +2405,7 @@
       <c r="S19">
         <v>9</v>
       </c>
-      <c r="T19" s="1" t="s">
+      <c r="T19" t="s">
         <v>111</v>
       </c>
       <c r="U19">
@@ -2451,7 +2415,7 @@
       <c r="AK19">
         <v>9</v>
       </c>
-      <c r="AL19" s="1" t="s">
+      <c r="AL19" t="s">
         <v>167</v>
       </c>
       <c r="AM19">
@@ -2461,15 +2425,15 @@
       <c r="AQ19">
         <v>9</v>
       </c>
-      <c r="AR19" s="1" t="s">
-        <v>180</v>
+      <c r="AR19" t="s">
+        <v>185</v>
       </c>
       <c r="AS19">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9</v>
       </c>
@@ -2483,7 +2447,7 @@
       <c r="G20">
         <v>9</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" t="s">
         <v>75</v>
       </c>
       <c r="I20">
@@ -2493,7 +2457,7 @@
       <c r="M20">
         <v>9</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="N20" t="s">
         <v>95</v>
       </c>
       <c r="O20">
@@ -2503,7 +2467,7 @@
       <c r="S20">
         <v>9</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="T20" t="s">
         <v>25</v>
       </c>
       <c r="U20">
@@ -2513,7 +2477,7 @@
       <c r="AK20">
         <v>9</v>
       </c>
-      <c r="AL20" s="1" t="s">
+      <c r="AL20" t="s">
         <v>160</v>
       </c>
       <c r="AM20">
@@ -2523,15 +2487,15 @@
       <c r="AQ20">
         <v>9</v>
       </c>
-      <c r="AR20" s="1" t="s">
-        <v>226</v>
+      <c r="AR20" t="s">
+        <v>171</v>
       </c>
       <c r="AS20">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9</v>
       </c>
@@ -2545,7 +2509,7 @@
       <c r="G21">
         <v>9</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" t="s">
         <v>76</v>
       </c>
       <c r="I21">
@@ -2555,7 +2519,7 @@
       <c r="M21">
         <v>9</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="N21" t="s">
         <v>39</v>
       </c>
       <c r="O21">
@@ -2565,7 +2529,7 @@
       <c r="S21">
         <v>9</v>
       </c>
-      <c r="T21" s="1" t="s">
+      <c r="T21" t="s">
         <v>112</v>
       </c>
       <c r="U21">
@@ -2575,7 +2539,7 @@
       <c r="AK21">
         <v>9</v>
       </c>
-      <c r="AL21" s="1" t="s">
+      <c r="AL21" t="s">
         <v>161</v>
       </c>
       <c r="AM21">
@@ -2585,19 +2549,19 @@
       <c r="AQ21">
         <v>9</v>
       </c>
-      <c r="AR21" s="1" t="s">
-        <v>225</v>
+      <c r="AR21" t="s">
+        <v>186</v>
       </c>
       <c r="AS21">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>28</v>
       </c>
       <c r="C22">
@@ -2607,7 +2571,7 @@
       <c r="G22">
         <v>9</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" t="s">
         <v>77</v>
       </c>
       <c r="I22">
@@ -2617,7 +2581,7 @@
       <c r="M22">
         <v>9</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="N22" t="s">
         <v>96</v>
       </c>
       <c r="O22">
@@ -2627,7 +2591,7 @@
       <c r="S22">
         <v>9</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="T22" t="s">
         <v>113</v>
       </c>
       <c r="U22">
@@ -2637,7 +2601,7 @@
       <c r="AK22">
         <v>9</v>
       </c>
-      <c r="AL22" s="1" t="s">
+      <c r="AL22" t="s">
         <v>162</v>
       </c>
       <c r="AM22">
@@ -2647,19 +2611,19 @@
       <c r="AQ22">
         <v>9</v>
       </c>
-      <c r="AR22" s="1" t="s">
-        <v>181</v>
+      <c r="AR22" t="s">
+        <v>187</v>
       </c>
       <c r="AS22">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>9</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>29</v>
       </c>
       <c r="C23">
@@ -2669,7 +2633,7 @@
       <c r="G23">
         <v>9</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" t="s">
         <v>78</v>
       </c>
       <c r="I23">
@@ -2679,7 +2643,7 @@
       <c r="M23">
         <v>9</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="N23" t="s">
         <v>97</v>
       </c>
       <c r="O23">
@@ -2699,7 +2663,7 @@
       <c r="AK23">
         <v>9</v>
       </c>
-      <c r="AL23" s="1" t="s">
+      <c r="AL23" t="s">
         <v>163</v>
       </c>
       <c r="AM23">
@@ -2709,19 +2673,19 @@
       <c r="AQ23">
         <v>9</v>
       </c>
-      <c r="AR23" s="1" t="s">
-        <v>182</v>
+      <c r="AR23" t="s">
+        <v>188</v>
       </c>
       <c r="AS23">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>30</v>
       </c>
       <c r="C24">
@@ -2731,7 +2695,7 @@
       <c r="G24">
         <v>9</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" t="s">
         <v>50</v>
       </c>
       <c r="I24">
@@ -2741,7 +2705,7 @@
       <c r="M24">
         <v>9</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="N24" t="s">
         <v>98</v>
       </c>
       <c r="O24">
@@ -2751,7 +2715,7 @@
       <c r="S24">
         <v>9</v>
       </c>
-      <c r="T24" s="1" t="s">
+      <c r="T24" t="s">
         <v>41</v>
       </c>
       <c r="U24">
@@ -2761,7 +2725,7 @@
       <c r="AK24">
         <v>9</v>
       </c>
-      <c r="AL24" s="1" t="s">
+      <c r="AL24" t="s">
         <v>164</v>
       </c>
       <c r="AM24">
@@ -2771,19 +2735,19 @@
       <c r="AQ24">
         <v>9</v>
       </c>
-      <c r="AR24" s="1" t="s">
-        <v>183</v>
+      <c r="AR24" t="s">
+        <v>189</v>
       </c>
       <c r="AS24">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>9</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>31</v>
       </c>
       <c r="C25">
@@ -2793,7 +2757,7 @@
       <c r="G25">
         <v>9</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" t="s">
         <v>79</v>
       </c>
       <c r="I25">
@@ -2803,7 +2767,7 @@
       <c r="M25">
         <v>9</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="N25" t="s">
         <v>99</v>
       </c>
       <c r="O25">
@@ -2813,7 +2777,7 @@
       <c r="S25">
         <v>9</v>
       </c>
-      <c r="T25" s="1" t="s">
+      <c r="T25" t="s">
         <v>115</v>
       </c>
       <c r="U25">
@@ -2833,15 +2797,15 @@
       <c r="AQ25">
         <v>9</v>
       </c>
-      <c r="AR25" s="1" t="s">
-        <v>184</v>
+      <c r="AR25" t="s">
+        <v>190</v>
       </c>
       <c r="AS25">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2855,7 +2819,7 @@
       <c r="S26">
         <v>9</v>
       </c>
-      <c r="T26" s="1" t="s">
+      <c r="T26" t="s">
         <v>114</v>
       </c>
       <c r="U26">
@@ -2865,15 +2829,15 @@
       <c r="AQ26">
         <v>17</v>
       </c>
-      <c r="AR26" s="1" t="s">
-        <v>185</v>
+      <c r="AR26" t="s">
+        <v>191</v>
       </c>
       <c r="AS26">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2887,7 +2851,7 @@
       <c r="S27">
         <v>9</v>
       </c>
-      <c r="T27" s="1" t="s">
+      <c r="T27" t="s">
         <v>116</v>
       </c>
       <c r="U27">
@@ -2897,15 +2861,15 @@
       <c r="AQ27">
         <v>17</v>
       </c>
-      <c r="AR27" s="1" t="s">
-        <v>186</v>
+      <c r="AR27" t="s">
+        <v>192</v>
       </c>
       <c r="AS27">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
@@ -2929,15 +2893,15 @@
       <c r="AQ28">
         <v>17</v>
       </c>
-      <c r="AR28" s="1" t="s">
-        <v>187</v>
+      <c r="AR28" t="s">
+        <v>193</v>
       </c>
       <c r="AS28">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>9</v>
       </c>
@@ -2961,15 +2925,15 @@
       <c r="AQ29">
         <v>17</v>
       </c>
-      <c r="AR29" s="1" t="s">
-        <v>188</v>
+      <c r="AR29" t="s">
+        <v>194</v>
       </c>
       <c r="AS29">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>9</v>
       </c>
@@ -2983,7 +2947,7 @@
       <c r="S30">
         <v>17</v>
       </c>
-      <c r="T30" s="1" t="s">
+      <c r="T30" t="s">
         <v>119</v>
       </c>
       <c r="U30">
@@ -2993,19 +2957,19 @@
       <c r="AQ30">
         <v>17</v>
       </c>
-      <c r="AR30" s="1" t="s">
-        <v>189</v>
+      <c r="AR30" t="s">
+        <v>195</v>
       </c>
       <c r="AS30">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>9</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>37</v>
       </c>
       <c r="C31">
@@ -3015,7 +2979,7 @@
       <c r="S31">
         <v>17</v>
       </c>
-      <c r="T31" s="1" t="s">
+      <c r="T31" t="s">
         <v>100</v>
       </c>
       <c r="U31">
@@ -3025,19 +2989,19 @@
       <c r="AQ31">
         <v>17</v>
       </c>
-      <c r="AR31" s="1" t="s">
-        <v>190</v>
+      <c r="AR31" t="s">
+        <v>196</v>
       </c>
       <c r="AS31">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>9</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>38</v>
       </c>
       <c r="C32">
@@ -3047,7 +3011,7 @@
       <c r="S32">
         <v>17</v>
       </c>
-      <c r="T32" s="1" t="s">
+      <c r="T32" t="s">
         <v>120</v>
       </c>
       <c r="U32">
@@ -3057,19 +3021,19 @@
       <c r="AQ32">
         <v>17</v>
       </c>
-      <c r="AR32" s="1" t="s">
-        <v>191</v>
+      <c r="AR32" t="s">
+        <v>197</v>
       </c>
       <c r="AS32">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>17</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>39</v>
       </c>
       <c r="C33">
@@ -3079,7 +3043,7 @@
       <c r="S33">
         <v>17</v>
       </c>
-      <c r="T33" s="1" t="s">
+      <c r="T33" t="s">
         <v>121</v>
       </c>
       <c r="U33">
@@ -3089,19 +3053,19 @@
       <c r="AQ33">
         <v>17</v>
       </c>
-      <c r="AR33" s="1" t="s">
-        <v>192</v>
+      <c r="AR33" t="s">
+        <v>198</v>
       </c>
       <c r="AS33">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>17</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>40</v>
       </c>
       <c r="C34">
@@ -3111,7 +3075,7 @@
       <c r="S34">
         <v>17</v>
       </c>
-      <c r="T34" s="1" t="s">
+      <c r="T34" t="s">
         <v>122</v>
       </c>
       <c r="U34">
@@ -3121,19 +3085,19 @@
       <c r="AQ34">
         <v>17</v>
       </c>
-      <c r="AR34" s="1" t="s">
-        <v>193</v>
+      <c r="AR34" t="s">
+        <v>199</v>
       </c>
       <c r="AS34">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>17</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>41</v>
       </c>
       <c r="C35">
@@ -3143,7 +3107,7 @@
       <c r="S35">
         <v>17</v>
       </c>
-      <c r="T35" s="1" t="s">
+      <c r="T35" t="s">
         <v>59</v>
       </c>
       <c r="U35">
@@ -3153,19 +3117,19 @@
       <c r="AQ35">
         <v>17</v>
       </c>
-      <c r="AR35" s="1" t="s">
-        <v>194</v>
+      <c r="AR35" t="s">
+        <v>200</v>
       </c>
       <c r="AS35">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>17</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>42</v>
       </c>
       <c r="C36">
@@ -3175,7 +3139,7 @@
       <c r="S36">
         <v>17</v>
       </c>
-      <c r="T36" s="1" t="s">
+      <c r="T36" t="s">
         <v>121</v>
       </c>
       <c r="U36">
@@ -3185,19 +3149,19 @@
       <c r="AQ36">
         <v>17</v>
       </c>
-      <c r="AR36" s="1" t="s">
-        <v>195</v>
+      <c r="AR36" t="s">
+        <v>201</v>
       </c>
       <c r="AS36">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>17</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>43</v>
       </c>
       <c r="C37">
@@ -3207,7 +3171,7 @@
       <c r="S37">
         <v>17</v>
       </c>
-      <c r="T37" s="1" t="s">
+      <c r="T37" t="s">
         <v>123</v>
       </c>
       <c r="U37">
@@ -3217,19 +3181,19 @@
       <c r="AQ37">
         <v>17</v>
       </c>
-      <c r="AR37" s="1" t="s">
-        <v>196</v>
+      <c r="AR37" t="s">
+        <v>202</v>
       </c>
       <c r="AS37">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>17</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>44</v>
       </c>
       <c r="C38">
@@ -3239,7 +3203,7 @@
       <c r="S38">
         <v>17</v>
       </c>
-      <c r="T38" s="1" t="s">
+      <c r="T38" t="s">
         <v>124</v>
       </c>
       <c r="U38">
@@ -3250,18 +3214,18 @@
         <v>17</v>
       </c>
       <c r="AR38" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="AS38">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>17</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>45</v>
       </c>
       <c r="C39">
@@ -3271,7 +3235,7 @@
       <c r="S39">
         <v>17</v>
       </c>
-      <c r="T39" s="1" t="s">
+      <c r="T39" t="s">
         <v>125</v>
       </c>
       <c r="U39">
@@ -3282,18 +3246,18 @@
         <v>17</v>
       </c>
       <c r="AR39" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="AS39">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>17</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>46</v>
       </c>
       <c r="C40">
@@ -3313,19 +3277,19 @@
       <c r="AQ40">
         <v>17</v>
       </c>
-      <c r="AR40" s="1" t="s">
-        <v>199</v>
+      <c r="AR40" t="s">
+        <v>205</v>
       </c>
       <c r="AS40">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>17</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>47</v>
       </c>
       <c r="C41">
@@ -3345,19 +3309,19 @@
       <c r="AQ41">
         <v>17</v>
       </c>
-      <c r="AR41" s="1" t="s">
-        <v>200</v>
+      <c r="AR41" t="s">
+        <v>206</v>
       </c>
       <c r="AS41">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>17</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>48</v>
       </c>
       <c r="C42">
@@ -3367,7 +3331,7 @@
       <c r="S42">
         <v>17</v>
       </c>
-      <c r="T42" s="1" t="s">
+      <c r="T42" t="s">
         <v>127</v>
       </c>
       <c r="U42">
@@ -3377,15 +3341,15 @@
       <c r="AQ42">
         <v>17</v>
       </c>
-      <c r="AR42" s="1" t="s">
-        <v>201</v>
+      <c r="AR42" t="s">
+        <v>207</v>
       </c>
       <c r="AS42">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>17</v>
       </c>
@@ -3399,7 +3363,7 @@
       <c r="S43">
         <v>17</v>
       </c>
-      <c r="T43" s="1" t="s">
+      <c r="T43" t="s">
         <v>128</v>
       </c>
       <c r="U43">
@@ -3409,15 +3373,15 @@
       <c r="AQ43">
         <v>17</v>
       </c>
-      <c r="AR43" s="1" t="s">
-        <v>202</v>
+      <c r="AR43" t="s">
+        <v>208</v>
       </c>
       <c r="AS43">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>17</v>
       </c>
@@ -3431,7 +3395,7 @@
       <c r="S44">
         <v>17</v>
       </c>
-      <c r="T44" s="1" t="s">
+      <c r="T44" t="s">
         <v>129</v>
       </c>
       <c r="U44">
@@ -3442,18 +3406,18 @@
         <v>17</v>
       </c>
       <c r="AR44" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="AS44">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>17</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>51</v>
       </c>
       <c r="C45">
@@ -3463,7 +3427,7 @@
       <c r="S45">
         <v>17</v>
       </c>
-      <c r="T45" s="1" t="s">
+      <c r="T45" t="s">
         <v>130</v>
       </c>
       <c r="U45">
@@ -3474,18 +3438,18 @@
         <v>17</v>
       </c>
       <c r="AR45" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="AS45">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>17</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>52</v>
       </c>
       <c r="C46">
@@ -3495,7 +3459,7 @@
       <c r="S46">
         <v>17</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="T46" t="s">
         <v>72</v>
       </c>
       <c r="U46">
@@ -3505,19 +3469,19 @@
       <c r="AQ46">
         <v>17</v>
       </c>
-      <c r="AR46" s="1" t="s">
-        <v>205</v>
+      <c r="AR46" t="s">
+        <v>211</v>
       </c>
       <c r="AS46">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>17</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>53</v>
       </c>
       <c r="C47">
@@ -3527,7 +3491,7 @@
       <c r="S47">
         <v>17</v>
       </c>
-      <c r="T47" s="1" t="s">
+      <c r="T47" t="s">
         <v>131</v>
       </c>
       <c r="U47">
@@ -3537,19 +3501,19 @@
       <c r="AQ47">
         <v>17</v>
       </c>
-      <c r="AR47" s="1" t="s">
-        <v>206</v>
+      <c r="AR47" t="s">
+        <v>212</v>
       </c>
       <c r="AS47">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>17</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>54</v>
       </c>
       <c r="C48">
@@ -3559,7 +3523,7 @@
       <c r="S48">
         <v>17</v>
       </c>
-      <c r="T48" s="1" t="s">
+      <c r="T48" t="s">
         <v>47</v>
       </c>
       <c r="U48">
@@ -3569,19 +3533,19 @@
       <c r="AQ48">
         <v>17</v>
       </c>
-      <c r="AR48" s="1" t="s">
-        <v>207</v>
+      <c r="AR48" t="s">
+        <v>213</v>
       </c>
       <c r="AS48">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>17</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>55</v>
       </c>
       <c r="C49">
@@ -3591,7 +3555,7 @@
       <c r="S49">
         <v>17</v>
       </c>
-      <c r="T49" s="1" t="s">
+      <c r="T49" t="s">
         <v>16</v>
       </c>
       <c r="U49">
@@ -3601,19 +3565,19 @@
       <c r="AQ49">
         <v>17</v>
       </c>
-      <c r="AR49" s="1" t="s">
-        <v>208</v>
+      <c r="AR49" t="s">
+        <v>214</v>
       </c>
       <c r="AS49">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>17</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>56</v>
       </c>
       <c r="C50">
@@ -3623,7 +3587,7 @@
       <c r="S50">
         <v>17</v>
       </c>
-      <c r="T50" s="1" t="s">
+      <c r="T50" t="s">
         <v>35</v>
       </c>
       <c r="U50">
@@ -3633,19 +3597,19 @@
       <c r="AQ50">
         <v>17</v>
       </c>
-      <c r="AR50" s="1" t="s">
-        <v>209</v>
+      <c r="AR50" t="s">
+        <v>215</v>
       </c>
       <c r="AS50">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>17</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>57</v>
       </c>
       <c r="C51">
@@ -3655,7 +3619,7 @@
       <c r="S51">
         <v>17</v>
       </c>
-      <c r="T51" s="1" t="s">
+      <c r="T51" t="s">
         <v>132</v>
       </c>
       <c r="U51">
@@ -3665,19 +3629,19 @@
       <c r="AQ51">
         <v>17</v>
       </c>
-      <c r="AR51" s="1" t="s">
-        <v>210</v>
+      <c r="AR51" t="s">
+        <v>216</v>
       </c>
       <c r="AS51">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>17</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>58</v>
       </c>
       <c r="C52">
@@ -3687,7 +3651,7 @@
       <c r="S52">
         <v>17</v>
       </c>
-      <c r="T52" s="1" t="s">
+      <c r="T52" t="s">
         <v>133</v>
       </c>
       <c r="U52">
@@ -3697,19 +3661,19 @@
       <c r="AQ52">
         <v>17</v>
       </c>
-      <c r="AR52" s="1" t="s">
-        <v>211</v>
+      <c r="AR52" t="s">
+        <v>217</v>
       </c>
       <c r="AS52">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.3">
       <c r="S53">
         <v>17</v>
       </c>
-      <c r="T53" s="1" t="s">
+      <c r="T53" t="s">
         <v>121</v>
       </c>
       <c r="U53">
@@ -3719,15 +3683,15 @@
       <c r="AQ53">
         <v>17</v>
       </c>
-      <c r="AR53" s="1" t="s">
-        <v>212</v>
+      <c r="AR53" t="s">
+        <v>218</v>
       </c>
       <c r="AS53">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -3737,7 +3701,7 @@
       <c r="S54">
         <v>17</v>
       </c>
-      <c r="T54" s="1" t="s">
+      <c r="T54" t="s">
         <v>105</v>
       </c>
       <c r="U54">
@@ -3747,15 +3711,15 @@
       <c r="AQ54">
         <v>17</v>
       </c>
-      <c r="AR54" s="1" t="s">
-        <v>213</v>
+      <c r="AR54" t="s">
+        <v>219</v>
       </c>
       <c r="AS54">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
@@ -3765,7 +3729,7 @@
       <c r="S55">
         <v>17</v>
       </c>
-      <c r="T55" s="1" t="s">
+      <c r="T55" t="s">
         <v>68</v>
       </c>
       <c r="U55">
@@ -3775,7 +3739,7 @@
       <c r="AQ55">
         <v>17</v>
       </c>
-      <c r="AR55" s="1" t="s">
+      <c r="AR55" t="s">
         <v>173</v>
       </c>
       <c r="AS55">
@@ -3783,7 +3747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3793,7 +3757,7 @@
       <c r="S56">
         <v>17</v>
       </c>
-      <c r="T56" s="1" t="s">
+      <c r="T56" t="s">
         <v>134</v>
       </c>
       <c r="U56">
@@ -3803,15 +3767,15 @@
       <c r="AQ56">
         <v>17</v>
       </c>
-      <c r="AR56" s="1" t="s">
-        <v>214</v>
+      <c r="AR56" t="s">
+        <v>220</v>
       </c>
       <c r="AS56">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>5</v>
       </c>
@@ -3821,7 +3785,7 @@
       <c r="S57">
         <v>17</v>
       </c>
-      <c r="T57" s="1" t="s">
+      <c r="T57" t="s">
         <v>79</v>
       </c>
       <c r="U57">
@@ -3831,15 +3795,15 @@
       <c r="AQ57">
         <v>17</v>
       </c>
-      <c r="AR57" s="1" t="s">
-        <v>209</v>
+      <c r="AR57" t="s">
+        <v>215</v>
       </c>
       <c r="AS57">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>9</v>
       </c>
@@ -3849,7 +3813,7 @@
       <c r="AQ58">
         <v>17</v>
       </c>
-      <c r="AR58" s="1" t="s">
+      <c r="AR58" t="s">
         <v>173</v>
       </c>
       <c r="AS58">
@@ -3857,7 +3821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>17</v>
       </c>
@@ -3867,19 +3831,19 @@
       <c r="AQ59">
         <v>17</v>
       </c>
-      <c r="AR59" s="1" t="s">
-        <v>215</v>
+      <c r="AR59" t="s">
+        <v>221</v>
       </c>
       <c r="AS59">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AQ60">
         <v>17</v>
       </c>
-      <c r="AR60" s="1" t="s">
+      <c r="AR60" t="s">
         <v>155</v>
       </c>
       <c r="AS60">
@@ -3887,12 +3851,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AQ61">
         <v>17</v>
       </c>
-      <c r="AR61" s="1" t="s">
-        <v>216</v>
+      <c r="AR61" t="s">
+        <v>222</v>
       </c>
       <c r="AS61">
         <f t="shared" si="6"/>

</xml_diff>